<commit_message>
Minor Clean-up of .ino file, adding licenses
</commit_message>
<xml_diff>
--- a/HELPStat/Software/Docs/HELPStat UUIDs.xlsx
+++ b/HELPStat/Software/Docs/HELPStat UUIDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3d19993c8b6b4d2/School/MedSchool/LinnesLab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="446" documentId="8_{88539AB8-C4C3-4A8A-8446-F1F72EFE6B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E15B2F2-6780-4B4B-981D-8B1297586412}"/>
+  <xr:revisionPtr revIDLastSave="451" documentId="8_{88539AB8-C4C3-4A8A-8446-F1F72EFE6B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19BDFB88-E452-4325-91D8-89FA4DFA5C89}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{FB397B27-D826-4B04-94BC-DE4CE3AECE45}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="9960" xr2:uid="{FB397B27-D826-4B04-94BC-DE4CE3AECE45}"/>
   </bookViews>
   <sheets>
     <sheet name="UUIDs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
   <si>
     <t>READ</t>
   </si>
@@ -667,6 +667,12 @@
   </si>
   <si>
     <t>Not Implemented</t>
+  </si>
+  <si>
+    <t>06192c1e-8588-4808-91b8-c4f1d650893d</t>
+  </si>
+  <si>
+    <t>Magnitude</t>
   </si>
 </sst>
 </file>
@@ -835,15 +841,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -863,20 +860,62 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -901,45 +940,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -978,6 +978,12 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -991,29 +997,28 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A021FDB-B380-4D73-811E-5F2F43FA34B4}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:E21" xr:uid="{1A021FDB-B380-4D73-811E-5F2F43FA34B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A021FDB-B380-4D73-811E-5F2F43FA34B4}" name="Table1" displayName="Table1" ref="A1:E22" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:E22" xr:uid="{1A021FDB-B380-4D73-811E-5F2F43FA34B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+    <sortCondition ref="A22"/>
+  </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5FB6EF75-6E9C-473B-8E45-837C8FA71172}" name="CHARACTERISTIC UUID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{4B8E2978-81E4-4034-AFEF-127EDCA771A1}" name="PARAMETER" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{5C41BBF0-2670-4486-84C6-83B74F3368C5}" name="NOTIFY" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BA05644A-8E9F-4F6B-BABC-380EE3877FD9}" name="READ" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5C41AF9C-EEC0-4CD1-895A-C569537495BE}" name="WRITE" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{5FB6EF75-6E9C-473B-8E45-837C8FA71172}" name="CHARACTERISTIC UUID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4B8E2978-81E4-4034-AFEF-127EDCA771A1}" name="PARAMETER" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5C41BBF0-2670-4486-84C6-83B74F3368C5}" name="NOTIFY" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{BA05644A-8E9F-4F6B-BABC-380EE3877FD9}" name="READ" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5C41AF9C-EEC0-4CD1-895A-C569537495BE}" name="WRITE" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A61F15CE-C4C0-469F-A22D-0637261D4EA9}" name="Table4" displayName="Table4" ref="G1:G5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A61F15CE-C4C0-469F-A22D-0637261D4EA9}" name="Table4" displayName="Table4" ref="G1:G5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="G1:G5" xr:uid="{A61F15CE-C4C0-469F-A22D-0637261D4EA9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{27991D30-5277-41CF-924F-54297A732E05}" name="LEGEND" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{27991D30-5277-41CF-924F-54297A732E05}" name="LEGEND" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1336,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAFD766-7698-4EC3-9F9F-0797B59D1714}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,257 +1358,268 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="18" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="15"/>
-      <c r="G2" s="18" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="12"/>
+      <c r="G2" s="15" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="10"/>
+      <c r="G3" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="G3" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="G4" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="15"/>
-      <c r="G4" s="20" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="12"/>
+      <c r="G5" s="19" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="15"/>
-      <c r="G5" s="22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
@@ -2643,7 +2659,7 @@
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="21" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2651,19 +2667,19 @@
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="20" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2671,13 +2687,13 @@
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -2722,7 +2738,7 @@
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="22" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2730,19 +2746,19 @@
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="21" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2750,19 +2766,19 @@
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2770,13 +2786,13 @@
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="22"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="22"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">

</xml_diff>